<commit_message>
updating fields returned by brazilcep on arrays that generate the dataframe
</commit_message>
<xml_diff>
--- a/lista_de_ceps_preenchidos.xlsx
+++ b/lista_de_ceps_preenchidos.xlsx
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>03275000</t>
+          <t>03275-000</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>03371020</t>
+          <t>03371-020</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">

</xml_diff>